<commit_message>
IMplemented reading from excel and writing into aggregated word table
</commit_message>
<xml_diff>
--- a/GenerateReport/ExcelTemplate.xlsx
+++ b/GenerateReport/ExcelTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adklinge\source\repos\GenerateReport\GenerateReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DABAB4F-C1DD-4B9C-AF3E-43D4405DFB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFBDFB2-A7D9-4DDE-983A-126685FF724C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{83AD150F-BCEF-4614-8A79-F436149B4AA6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>מספר סידורי</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>אלה אטלנטית</t>
+  </si>
+  <si>
+    <t>אלון</t>
   </si>
 </sst>
 </file>
@@ -117,21 +120,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,120 +450,147 @@
   <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="19.41796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.26171875" style="1" customWidth="1"/>
-    <col min="3" max="5" width="8.83984375" style="1"/>
-    <col min="6" max="6" width="11.68359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.15625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.3671875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.89453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.15625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.1015625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.83984375" style="1"/>
-    <col min="14" max="15" width="13.1015625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="1" width="19.41796875" customWidth="1"/>
+    <col min="2" max="2" width="25.26171875" customWidth="1"/>
+    <col min="6" max="6" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.15625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.3671875" customWidth="1"/>
+    <col min="9" max="9" width="13.89453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.15625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1015625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="13.1015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2">
         <v>3.3</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2">
         <v>2</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2">
         <v>3</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2">
         <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D3">
+        <v>6.44</v>
+      </c>
+      <c r="E3">
+        <v>1.5</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>2000</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="J5" s="2"/>
+      <c r="J5" s="1"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="P21" s="3"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="P21" s="2"/>
     </row>
     <row r="44" spans="2:9" ht="16.8" x14ac:dyDescent="0.65">
-      <c r="B44" s="4"/>
-      <c r="I44" s="5"/>
+      <c r="B44" s="3"/>
+      <c r="I44" s="4"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="I45" s="3"/>
+      <c r="I45" s="2"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B49" s="6"/>
+      <c r="B49" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -571,6 +599,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -579,15 +616,6 @@
     <MediaServiceKeyPoints xmlns="b0ccb347-d89b-4a48-8ba5-b466c519a984" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -867,6 +895,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A28702E4-405C-4146-90B6-2695D9BD928C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EDBCAC5-14E0-445F-BD62-0DFE0E2C1498}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -880,14 +916,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A28702E4-405C-4146-90B6-2695D9BD928C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>